<commit_message>
detailed control : climax music : so that voice can be heard clearly
</commit_message>
<xml_diff>
--- a/LedLight_Kanda.xlsx
+++ b/LedLight_Kanda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="1180" windowWidth="33180" windowHeight="22200" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2860" yWindow="1180" windowWidth="33180" windowHeight="22200" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="1" r:id="rId1"/>
@@ -5785,7 +5785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A60" zoomScale="75" workbookViewId="0">
       <selection sqref="A1:XFD108"/>
     </sheetView>
   </sheetViews>
@@ -6773,7 +6773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>